<commit_message>
adding high dim contractions
</commit_message>
<xml_diff>
--- a/high_dim_con.xlsx
+++ b/high_dim_con.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srinath/Documents/GitHub/cuda_python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E3C4E5F-2490-7743-9A08-A75544050556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1E4C65-7700-0442-8175-36E09DC5D433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{E3220547-C2A3-8B4E-97D6-08DE130750E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="81">
   <si>
     <t>adim</t>
   </si>
@@ -119,27 +119,12 @@
     <t>abc * cde -&gt; abde-fp16</t>
   </si>
   <si>
-    <t>(20, 16, 20)</t>
-  </si>
-  <si>
-    <t>(16, 20)</t>
-  </si>
-  <si>
     <t>(16, 16, 20)</t>
   </si>
   <si>
-    <t>ab * bde -&gt; abde-fp32</t>
-  </si>
-  <si>
-    <t>ab * bde -&gt; abde-fp16</t>
-  </si>
-  <si>
     <t>([1], [1])</t>
   </si>
   <si>
-    <t>ab * bde -&gt; ade</t>
-  </si>
-  <si>
     <t>(20, 12, 20)</t>
   </si>
   <si>
@@ -164,12 +149,6 @@
     <t>ab * bcde -&gt; acde-fp16</t>
   </si>
   <si>
-    <t>(20, 12, 16, 16)</t>
-  </si>
-  <si>
-    <t>(4096, 12, 16, 16)</t>
-  </si>
-  <si>
     <t>(20, 8, 8, 20)</t>
   </si>
   <si>
@@ -201,13 +180,112 @@
   </si>
   <si>
     <t>abc * ebc -&gt; ae-fp16</t>
+  </si>
+  <si>
+    <t>(120, 200)</t>
+  </si>
+  <si>
+    <t>(200, 80, 200)</t>
+  </si>
+  <si>
+    <t>(120, 80, 200)</t>
+  </si>
+  <si>
+    <t>(1200, 2000)</t>
+  </si>
+  <si>
+    <t>(2000, 800, 2000)</t>
+  </si>
+  <si>
+    <t>(1200, 800, 2000)</t>
+  </si>
+  <si>
+    <t>(200,0 8, 200)</t>
+  </si>
+  <si>
+    <t>(120, 80, 80, 200)</t>
+  </si>
+  <si>
+    <t>(1200, 800, 800, 2000)</t>
+  </si>
+  <si>
+    <t>(160, 160, 200)</t>
+  </si>
+  <si>
+    <t>(200, 120, 200)</t>
+  </si>
+  <si>
+    <t>(160, 160, 120, 200)</t>
+  </si>
+  <si>
+    <t>(1600, 1600, 2000)</t>
+  </si>
+  <si>
+    <t>(2000, 1200, 2000)</t>
+  </si>
+  <si>
+    <t>(1600, 1600, 1200, 2000)</t>
+  </si>
+  <si>
+    <t>(320, 200)</t>
+  </si>
+  <si>
+    <t>(200, 80, 80, 120)</t>
+  </si>
+  <si>
+    <t>(320, 80, 80, 120)</t>
+  </si>
+  <si>
+    <t>(3200, 2000)</t>
+  </si>
+  <si>
+    <t>(2000, 800, 800, 1200)</t>
+  </si>
+  <si>
+    <t>(3200, 800, 800, 1200)</t>
+  </si>
+  <si>
+    <t>(40960, 7680)</t>
+  </si>
+  <si>
+    <t>(200, 7680)</t>
+  </si>
+  <si>
+    <t>(40960, 200)</t>
+  </si>
+  <si>
+    <t>(409600, 76800)</t>
+  </si>
+  <si>
+    <t>(2000, 76800)</t>
+  </si>
+  <si>
+    <t>(409600, 2000)</t>
+  </si>
+  <si>
+    <t>(200, 80, 80, 200)</t>
+  </si>
+  <si>
+    <t>(2000, 800, 800, 2000)</t>
+  </si>
+  <si>
+    <t>(120, 640, 200)</t>
+  </si>
+  <si>
+    <t>(200, 640, 200)</t>
+  </si>
+  <si>
+    <t>(1200, 6400, 2000)</t>
+  </si>
+  <si>
+    <t>(2000, 6400, 2000)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -239,6 +317,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -260,11 +345,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,14 +665,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533FA1DA-7CC0-DB47-8E54-9F4B65E35022}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
     <col min="5" max="5" width="19.1640625" customWidth="1"/>
     <col min="7" max="7" width="27.5" customWidth="1"/>
   </cols>
@@ -661,109 +750,109 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="A4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>24</v>
+      <c r="E4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="A5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>26</v>
+      <c r="E5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>30</v>
+      <c r="A6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>31</v>
+      <c r="A7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>23</v>
@@ -777,16 +866,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>23</v>
@@ -800,232 +889,784 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>14</v>
+      <c r="A12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>18</v>
+      <c r="A13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="1" t="s">
+      <c r="E32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="F38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="1" t="s">
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="1" t="s">
+      <c r="E39" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="F40" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="1" t="s">
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" s="1" t="s">
+      <c r="E41" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="D42" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>54</v>
+      <c r="D43" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correcting list of cons
</commit_message>
<xml_diff>
--- a/high_dim_con.xlsx
+++ b/high_dim_con.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srinath/Documents/GitHub/cuda_python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1E4C65-7700-0442-8175-36E09DC5D433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD311DD3-85AC-AE4E-84E3-CF924FF15334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{E3220547-C2A3-8B4E-97D6-08DE130750E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="80">
   <si>
     <t>adim</t>
   </si>
@@ -198,9 +198,6 @@
   </si>
   <si>
     <t>(1200, 800, 2000)</t>
-  </si>
-  <si>
-    <t>(200,0 8, 200)</t>
   </si>
   <si>
     <t>(120, 80, 80, 200)</t>
@@ -667,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533FA1DA-7CC0-DB47-8E54-9F4B65E35022}">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="166" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -892,10 +889,10 @@
         <v>50</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>22</v>
@@ -918,7 +915,7 @@
         <v>49</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>22</v>
@@ -941,7 +938,7 @@
         <v>52</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>22</v>
@@ -964,7 +961,7 @@
         <v>52</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>22</v>
@@ -1027,13 +1024,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>17</v>
@@ -1050,13 +1047,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>17</v>
@@ -1073,13 +1070,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>17</v>
@@ -1096,13 +1093,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>17</v>
@@ -1165,13 +1162,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>17</v>
@@ -1188,13 +1185,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>17</v>
@@ -1211,13 +1208,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>17</v>
@@ -1234,13 +1231,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>17</v>
@@ -1303,13 +1300,13 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>28</v>
@@ -1326,13 +1323,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>28</v>
@@ -1349,13 +1346,13 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>28</v>
@@ -1372,13 +1369,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>28</v>
@@ -1441,7 +1438,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>49</v>
@@ -1464,7 +1461,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>49</v>
@@ -1487,7 +1484,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>52</v>
@@ -1510,7 +1507,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>52</v>
@@ -1579,10 +1576,10 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>48</v>
@@ -1602,10 +1599,10 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>48</v>
@@ -1625,10 +1622,10 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>51</v>
@@ -1648,10 +1645,10 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
trying other high dim contractions
</commit_message>
<xml_diff>
--- a/high_dim_con.xlsx
+++ b/high_dim_con.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srinath/Documents/GitHub/cuda_python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD311DD3-85AC-AE4E-84E3-CF924FF15334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0FF6FD-A6C2-A047-A920-EEA3EA945289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{E3220547-C2A3-8B4E-97D6-08DE130750E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="96">
   <si>
     <t>adim</t>
   </si>
@@ -276,6 +276,54 @@
   </si>
   <si>
     <t>(2000, 6400, 2000)</t>
+  </si>
+  <si>
+    <t>(1200, 200)</t>
+  </si>
+  <si>
+    <t>(200, 800, 200)</t>
+  </si>
+  <si>
+    <t>(1200, 800, 200)</t>
+  </si>
+  <si>
+    <t>(1200, 800, 800, 200)</t>
+  </si>
+  <si>
+    <t>(1600, 1600, 200)</t>
+  </si>
+  <si>
+    <t>(200, 1200, 200)</t>
+  </si>
+  <si>
+    <t>(1600, 1600, 1200, 200)</t>
+  </si>
+  <si>
+    <t>(3200, 200)</t>
+  </si>
+  <si>
+    <t>(200, 800, 800, 120)</t>
+  </si>
+  <si>
+    <t>(3200, 800, 800, 120)</t>
+  </si>
+  <si>
+    <t>(2000, 7680)</t>
+  </si>
+  <si>
+    <t>(40960, 2000)</t>
+  </si>
+  <si>
+    <t>(2000, 800, 80, 200)</t>
+  </si>
+  <si>
+    <t>(2000, 80, 200)</t>
+  </si>
+  <si>
+    <t>(1200, 640, 200)</t>
+  </si>
+  <si>
+    <t>(2000, 640, 200)</t>
   </si>
 </sst>
 </file>
@@ -662,16 +710,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533FA1DA-7CC0-DB47-8E54-9F4B65E35022}">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="166" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="166" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
     <col min="5" max="5" width="19.1640625" customWidth="1"/>
     <col min="7" max="7" width="27.5" customWidth="1"/>
@@ -839,60 +887,60 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="A8" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>24</v>
+      <c r="E8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="A9" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>26</v>
+      <c r="E9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>22</v>
@@ -909,13 +957,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>22</v>
@@ -932,13 +980,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>22</v>
@@ -955,13 +1003,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>22</v>
@@ -978,16 +1026,16 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>23</v>
@@ -1001,16 +1049,16 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>23</v>
@@ -1024,16 +1072,16 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>23</v>
@@ -1047,16 +1095,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>23</v>
@@ -1070,13 +1118,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>17</v>
@@ -1093,13 +1141,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>17</v>
@@ -1116,553 +1164,875 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G25" s="1" t="s">
+      <c r="F26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G26" s="2" t="s">
+      <c r="F34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27" s="2" t="s">
+      <c r="F35" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G28" s="2" t="s">
+      <c r="F36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" s="2" t="s">
+      <c r="F37" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G37" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G30" s="2" t="s">
+      <c r="F38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G31" s="2" t="s">
+      <c r="F39" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G32" s="1" t="s">
+      <c r="F42" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G33" s="1" t="s">
+      <c r="F43" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G43" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G34" s="1" t="s">
+      <c r="F44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G35" s="1" t="s">
+      <c r="F45" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G36" s="1" t="s">
+      <c r="F46" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G46" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F37" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G37" s="1" t="s">
+      <c r="F47" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G47" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C50" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E50" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G38" s="1" t="s">
+      <c r="F50" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C51" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F39" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G39" s="1" t="s">
+      <c r="F51" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G51" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>76</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C52" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F40" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G40" s="1" t="s">
+      <c r="F52" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G52" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>76</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C53" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E53" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F41" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G41" s="1" t="s">
+      <c r="F53" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>78</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C54" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F42" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G42" s="1" t="s">
+      <c r="F54" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G54" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>78</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C55" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E55" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F43" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G43" s="1" t="s">
+      <c r="F55" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>94</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>94</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G57" s="1" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Trying slightly different dimensions
</commit_message>
<xml_diff>
--- a/high_dim_con.xlsx
+++ b/high_dim_con.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srinath/Documents/GitHub/cuda_python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0FF6FD-A6C2-A047-A920-EEA3EA945289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA6A612-D17F-154F-ADED-50A55DC6F356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{E3220547-C2A3-8B4E-97D6-08DE130750E0}"/>
+    <workbookView xWindow="6520" yWindow="2460" windowWidth="30240" windowHeight="18880" xr2:uid="{E3220547-C2A3-8B4E-97D6-08DE130750E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="112">
   <si>
     <t>adim</t>
   </si>
@@ -324,6 +324,54 @@
   </si>
   <si>
     <t>(2000, 640, 200)</t>
+  </si>
+  <si>
+    <t>(250, 160, 200)</t>
+  </si>
+  <si>
+    <t>(200, 200, 200)</t>
+  </si>
+  <si>
+    <t>(150, 160, 200, 200)</t>
+  </si>
+  <si>
+    <t>(160, 160, 200, 200)</t>
+  </si>
+  <si>
+    <t>(4096, 12, 12, 8)</t>
+  </si>
+  <si>
+    <t>(12, 12, 8, 300)</t>
+  </si>
+  <si>
+    <t>(4096, 300)</t>
+  </si>
+  <si>
+    <t>([1,2,3], [0,1,2])</t>
+  </si>
+  <si>
+    <t>abcd * bcde -&gt; ae</t>
+  </si>
+  <si>
+    <t>abcd * bcde -&gt; ae-fp32</t>
+  </si>
+  <si>
+    <t>abcd * bcde -&gt; ae-fp16</t>
+  </si>
+  <si>
+    <t>(12, 12, 8, 4096)</t>
+  </si>
+  <si>
+    <t>abcd * abce -&gt; ae</t>
+  </si>
+  <si>
+    <t>([0,1,2], [0,1,2])</t>
+  </si>
+  <si>
+    <t>abcd * abce -&gt; ae-fp32</t>
+  </si>
+  <si>
+    <t>abcd * abce -&gt; ae-fp16</t>
   </si>
 </sst>
 </file>
@@ -710,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533FA1DA-7CC0-DB47-8E54-9F4B65E35022}">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="166" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="166" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1210,13 +1258,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>59</v>
+        <v>96</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>60</v>
+        <v>97</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>61</v>
+        <v>98</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>17</v>
@@ -1233,13 +1281,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>59</v>
+        <v>96</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>60</v>
+        <v>97</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>17</v>
@@ -1256,13 +1304,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>17</v>
@@ -1279,13 +1327,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>17</v>
@@ -1302,59 +1350,59 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>17</v>
@@ -1371,13 +1419,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>17</v>
@@ -1394,13 +1442,13 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>17</v>
@@ -1417,13 +1465,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>17</v>
@@ -1440,13 +1488,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>17</v>
@@ -1463,13 +1511,13 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>17</v>
@@ -1485,60 +1533,60 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>14</v>
+      <c r="A34" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>18</v>
+      <c r="A35" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>68</v>
+        <v>10</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>28</v>
@@ -1555,13 +1603,13 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>68</v>
+        <v>10</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>28</v>
@@ -1578,13 +1626,13 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>28</v>
@@ -1601,13 +1649,13 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>28</v>
@@ -1624,13 +1672,13 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>28</v>
@@ -1647,13 +1695,13 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>28</v>
@@ -1669,60 +1717,60 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>38</v>
+      <c r="A42" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G42" s="1" t="s">
-        <v>40</v>
+      <c r="G42" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>38</v>
+      <c r="A43" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G43" s="1" t="s">
-        <v>41</v>
+      <c r="G43" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>39</v>
@@ -1739,13 +1787,13 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>39</v>
@@ -1762,13 +1810,13 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>39</v>
@@ -1785,13 +1833,13 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>39</v>
@@ -1808,10 +1856,10 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>93</v>
+        <v>52</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>52</v>
@@ -1831,10 +1879,10 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>93</v>
+        <v>52</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>52</v>
@@ -1853,60 +1901,60 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>42</v>
+      <c r="A50" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>25</v>
+        <v>93</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>42</v>
+      <c r="A51" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>25</v>
+        <v>93</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>45</v>
@@ -1923,13 +1971,13 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>45</v>
@@ -1946,13 +1994,13 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>45</v>
@@ -1969,13 +2017,13 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>45</v>
@@ -1992,10 +2040,10 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>51</v>
@@ -2015,10 +2063,10 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>51</v>
@@ -2034,6 +2082,144 @@
       </c>
       <c r="G57" s="1" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>94</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>94</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>100</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>100</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>107</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>107</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trying littel higher dims
</commit_message>
<xml_diff>
--- a/high_dim_con.xlsx
+++ b/high_dim_con.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srinath/Documents/GitHub/cuda_python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA6A612-D17F-154F-ADED-50A55DC6F356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E6B5BB-0527-7C46-B4D0-93040190FACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6520" yWindow="2460" windowWidth="30240" windowHeight="18880" xr2:uid="{E3220547-C2A3-8B4E-97D6-08DE130750E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="114">
   <si>
     <t>adim</t>
   </si>
@@ -332,12 +332,6 @@
     <t>(200, 200, 200)</t>
   </si>
   <si>
-    <t>(150, 160, 200, 200)</t>
-  </si>
-  <si>
-    <t>(160, 160, 200, 200)</t>
-  </si>
-  <si>
     <t>(4096, 12, 12, 8)</t>
   </si>
   <si>
@@ -372,6 +366,18 @@
   </si>
   <si>
     <t>abcd * abce -&gt; ae-fp16</t>
+  </si>
+  <si>
+    <t>(400, 160, 200)</t>
+  </si>
+  <si>
+    <t>(200, 200, 400)</t>
+  </si>
+  <si>
+    <t>(250, 160, 200, 200)</t>
+  </si>
+  <si>
+    <t>(400, 160, 200, 400)</t>
   </si>
 </sst>
 </file>
@@ -758,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533FA1DA-7CC0-DB47-8E54-9F4B65E35022}">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="166" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="166" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1264,7 +1270,7 @@
         <v>97</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>17</v>
@@ -1287,7 +1293,7 @@
         <v>97</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>17</v>
@@ -1304,13 +1310,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>60</v>
+        <v>111</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>61</v>
+        <v>113</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>17</v>
@@ -1327,13 +1333,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>60</v>
+        <v>111</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>61</v>
+        <v>113</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>17</v>
@@ -1350,13 +1356,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>17</v>
@@ -1373,13 +1379,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>17</v>
@@ -1396,59 +1402,59 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>17</v>
@@ -1465,13 +1471,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>17</v>
@@ -1488,13 +1494,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>17</v>
@@ -1511,13 +1517,13 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>17</v>
@@ -1534,13 +1540,13 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>17</v>
@@ -1557,13 +1563,13 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>17</v>
@@ -1579,60 +1585,60 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>14</v>
+      <c r="A36" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>18</v>
+      <c r="A37" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>68</v>
+        <v>10</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>28</v>
@@ -1649,13 +1655,13 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>68</v>
+        <v>10</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>28</v>
@@ -1672,13 +1678,13 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>28</v>
@@ -1695,13 +1701,13 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>28</v>
@@ -1718,13 +1724,13 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>28</v>
@@ -1741,13 +1747,13 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>28</v>
@@ -1763,60 +1769,60 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>38</v>
+      <c r="A44" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G44" s="1" t="s">
-        <v>40</v>
+      <c r="G44" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>38</v>
+      <c r="A45" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G45" s="1" t="s">
-        <v>41</v>
+      <c r="G45" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>39</v>
@@ -1833,13 +1839,13 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>39</v>
@@ -1856,13 +1862,13 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>39</v>
@@ -1879,13 +1885,13 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>39</v>
@@ -1902,10 +1908,10 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>93</v>
+        <v>52</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>52</v>
@@ -1925,10 +1931,10 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>93</v>
+        <v>52</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>52</v>
@@ -1947,60 +1953,60 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>42</v>
+      <c r="A52" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>25</v>
+        <v>93</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>42</v>
+      <c r="A53" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>25</v>
+        <v>93</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>45</v>
@@ -2017,13 +2023,13 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>45</v>
@@ -2040,13 +2046,13 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>45</v>
@@ -2063,13 +2069,13 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>45</v>
@@ -2086,10 +2092,10 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>51</v>
@@ -2109,10 +2115,10 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>51</v>
@@ -2132,94 +2138,140 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>102</v>
+        <v>51</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>103</v>
+        <v>45</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>104</v>
+        <v>44</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>105</v>
+        <v>46</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>102</v>
+        <v>51</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>103</v>
+        <v>45</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>104</v>
+        <v>44</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>106</v>
+        <v>47</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B62" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="E62" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="F62" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>98</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>105</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D63" s="1" t="s">
+      <c r="E64" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>105</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G65" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trying little higher dims
</commit_message>
<xml_diff>
--- a/high_dim_con.xlsx
+++ b/high_dim_con.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srinath/Documents/GitHub/cuda_python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E6B5BB-0527-7C46-B4D0-93040190FACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414BE35F-C41B-9244-B5A1-764B97C54F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6520" yWindow="2460" windowWidth="30240" windowHeight="18880" xr2:uid="{E3220547-C2A3-8B4E-97D6-08DE130750E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="117">
   <si>
     <t>adim</t>
   </si>
@@ -378,6 +378,15 @@
   </si>
   <si>
     <t>(400, 160, 200, 400)</t>
+  </si>
+  <si>
+    <t>(300, 160, 200)</t>
+  </si>
+  <si>
+    <t>(200, 200, 300)</t>
+  </si>
+  <si>
+    <t>(300, 160, 200, 300)</t>
   </si>
 </sst>
 </file>
@@ -764,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533FA1DA-7CC0-DB47-8E54-9F4B65E35022}">
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" zoomScale="166" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1310,13 +1319,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>17</v>
@@ -1333,13 +1342,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>17</v>
@@ -1356,13 +1365,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>60</v>
+        <v>111</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>61</v>
+        <v>113</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>17</v>
@@ -1379,13 +1388,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>60</v>
+        <v>111</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>61</v>
+        <v>113</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>17</v>
@@ -1402,13 +1411,13 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>17</v>
@@ -1425,13 +1434,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>17</v>
@@ -1448,59 +1457,59 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>17</v>
@@ -1517,13 +1526,13 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>17</v>
@@ -1540,13 +1549,13 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>17</v>
@@ -1563,13 +1572,13 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>17</v>
@@ -1586,13 +1595,13 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>17</v>
@@ -1609,13 +1618,13 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>17</v>
@@ -1631,60 +1640,60 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>14</v>
+      <c r="A38" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>18</v>
+      <c r="A39" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>68</v>
+        <v>10</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>28</v>
@@ -1701,13 +1710,13 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>68</v>
+        <v>10</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>28</v>
@@ -1724,13 +1733,13 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>28</v>
@@ -1747,13 +1756,13 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>28</v>
@@ -1770,13 +1779,13 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>28</v>
@@ -1793,13 +1802,13 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>28</v>
@@ -1815,60 +1824,60 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>38</v>
+      <c r="A46" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G46" s="1" t="s">
-        <v>40</v>
+      <c r="G46" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>38</v>
+      <c r="A47" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G47" s="1" t="s">
-        <v>41</v>
+      <c r="G47" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>39</v>
@@ -1885,13 +1894,13 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>39</v>
@@ -1908,13 +1917,13 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>39</v>
@@ -1931,13 +1940,13 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>39</v>
@@ -1954,10 +1963,10 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>93</v>
+        <v>52</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>52</v>
@@ -1977,10 +1986,10 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>93</v>
+        <v>52</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>52</v>
@@ -1999,60 +2008,60 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>42</v>
+      <c r="A54" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>25</v>
+        <v>93</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>42</v>
+      <c r="A55" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>25</v>
+        <v>93</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>45</v>
@@ -2069,13 +2078,13 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>45</v>
@@ -2092,13 +2101,13 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>45</v>
@@ -2115,13 +2124,13 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>45</v>
@@ -2138,10 +2147,10 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>51</v>
@@ -2161,10 +2170,10 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>51</v>
@@ -2184,53 +2193,53 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>100</v>
+        <v>51</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>102</v>
+        <v>44</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>103</v>
+        <v>46</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>100</v>
+        <v>51</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>102</v>
+        <v>44</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>104</v>
+        <v>47</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>99</v>
@@ -2239,21 +2248,21 @@
         <v>100</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>99</v>
@@ -2262,15 +2271,61 @@
         <v>100</v>
       </c>
       <c r="D65" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>105</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E65" s="1" t="s">
+      <c r="E66" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F65" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G65" s="1" t="s">
+      <c r="F66" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>105</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G67" s="1" t="s">
         <v>109</v>
       </c>
     </row>

</xml_diff>